<commit_message>
Refactor: create getRandomLocation function
</commit_message>
<xml_diff>
--- a/data/VolarisTestData.xlsx
+++ b/data/VolarisTestData.xlsx
@@ -103,16 +103,16 @@
     <t>Mexico City (All airports)</t>
   </si>
   <si>
+    <t>Morelia</t>
+  </si>
+  <si>
     <t>Monterrey</t>
   </si>
   <si>
-    <t>Morelia</t>
+    <t>Oaxaca</t>
   </si>
   <si>
     <t>Puebla</t>
-  </si>
-  <si>
-    <t>Oaxaca</t>
   </si>
   <si>
     <t>Puerto Escondido</t>
@@ -225,9 +225,6 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
@@ -290,7 +287,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -298,7 +295,7 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
@@ -306,7 +303,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13">
@@ -314,7 +311,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14">
@@ -322,7 +319,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15">
@@ -330,7 +327,7 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16">
@@ -338,7 +335,7 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17">
@@ -346,7 +343,7 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18">
@@ -354,7 +351,7 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19">
@@ -362,7 +359,7 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20">
@@ -370,7 +367,7 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21">
@@ -378,7 +375,7 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22">
@@ -386,7 +383,7 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23">
@@ -394,7 +391,7 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24">
@@ -402,7 +399,7 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25">
@@ -410,7 +407,7 @@
         <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26">
@@ -418,7 +415,7 @@
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27">
@@ -431,23 +428,23 @@
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
         <v>34</v>
@@ -455,7 +452,7 @@
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
         <v>35</v>

</xml_diff>